<commit_message>
Ajout données sur les sols
</commit_message>
<xml_diff>
--- a/Sol.xlsx
+++ b/Sol.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -16,6 +16,44 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+  <si>
+    <t>N° segment</t>
+  </si>
+  <si>
+    <t>pièce</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>couleur</t>
+  </si>
+  <si>
+    <t>surface</t>
+  </si>
+  <si>
+    <t>Salle</t>
+  </si>
+  <si>
+    <t>cuisine</t>
+  </si>
+  <si>
+    <t>chambre 1</t>
+  </si>
+  <si>
+    <t>carrelage</t>
+  </si>
+  <si>
+    <t>salle de bains</t>
+  </si>
+  <si>
+    <t>parquet</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -331,12 +369,170 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>